<commit_message>
Revert back CosMx Transcriptomics v2 to its original state
</commit_message>
<xml_diff>
--- a/cosmx-transcriptomics/v2.0.0/cosmx-transcriptomics-v2.0.0.xlsx
+++ b/cosmx-transcriptomics/v2.0.0/cosmx-transcriptomics-v2.0.0.xlsx
@@ -247,20 +247,6 @@
     </comment>
     <comment ref="AF1" authorId="1">
       <text>
-        <t>A semicolon separated list of non-shared files to be included in the dataset.
-The path assumes the files are located in the "TOP/non-global/" directory. For
-example, for the file is
-TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
-field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
-these files will be copied to the appropriate locations within the respective
-dataset directory tree. This field is used for internal HuBMAP processing.
-Examples for GeoMx and PhenoCycler are provided in the File Locations
-documentation:
-https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
-      </text>
-    </comment>
-    <comment ref="AG1" authorId="1">
-      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -271,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="449">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1593,9 +1579,6 @@
     <t>anatomical_structure_id</t>
   </si>
   <si>
-    <t>non_global_files</t>
-  </si>
-  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1614,7 +1597,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-09-18T09:01:55-07:00</t>
+    <t>2025-09-18T12:34:44-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1673,7 +1656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -1710,7 +1693,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1721,7 +1703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1758,8 +1740,7 @@
     <col min="29" max="29" style="30" width="7.4296875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" style="31" width="21.44921875" customWidth="true" bestFit="true"/>
     <col min="31" max="31" style="32" width="19.23828125" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" style="33" width="13.33984375" customWidth="true" bestFit="true"/>
-    <col min="33" max="33" style="34" width="16.91796875" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" style="33" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1859,16 +1840,13 @@
       <c r="AF1" t="s" s="1">
         <v>440</v>
       </c>
-      <c r="AG1" t="s" s="1">
-        <v>441</v>
-      </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="AG2" t="s" s="34">
-        <v>442</v>
+      <c r="AF2" t="s" s="33">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -2294,16 +2272,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
+        <v>442</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>443</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>444</v>
-      </c>
       <c r="C1" t="s" s="0">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2">
@@ -2311,13 +2289,13 @@
         <v>24</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>